<commit_message>
making sure it's up to date
</commit_message>
<xml_diff>
--- a/sources.xlsx
+++ b/sources.xlsx
@@ -804,9 +804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +815,10 @@
     <col min="2" max="2" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="5" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="62.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -848,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>30</v>
       </c>
@@ -888,7 +888,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>32</v>
       </c>
@@ -908,7 +908,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>83</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>87</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>103</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>86</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
@@ -1173,491 +1173,491 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1976</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1977</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1403992</v>
+      </c>
+      <c r="B18" s="1">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1994</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>3452230</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B23" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D23" s="1">
         <v>1971</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1976</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1977</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>33</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1977</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1">
-        <v>16</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1979</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1981</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1983</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="1">
-        <v>35</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1983</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1">
-        <v>1986</v>
+        <v>1977</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1">
-        <v>1991</v>
+        <v>1979</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D26" s="1">
-        <v>1992</v>
+        <v>1981</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>1403992</v>
+        <v>54</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B27" s="1">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1">
-        <v>1994</v>
+        <v>1983</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="B28" s="1">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="D28" s="1">
-        <v>2001</v>
+        <v>1983</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="B29" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D29" s="1">
-        <v>2002</v>
+        <v>1986</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D30" s="1">
+        <v>1991</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="1">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1992</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="1">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
         <v>2002</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="1">
-        <v>27</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2003</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2003</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>2188261</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2006</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>2188261</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2006</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>3452230</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="B35" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>3407494</v>
       </c>
@@ -1685,7 +1685,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:H36">
-    <sortCondition ref="D1"/>
+    <sortCondition ref="E1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
saved the file first. that helped. :^)
</commit_message>
<xml_diff>
--- a/sources.xlsx
+++ b/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5535" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="166">
   <si>
     <t>ref</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Schroer, B.</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Simmons, G.</t>
   </si>
   <si>
@@ -474,6 +471,57 @@
   </si>
   <si>
     <t>Robert E. Krieger Publishing Co., Inc., Melbourne, Fla., 1983.</t>
+  </si>
+  <si>
+    <t>Lin, H.; Niu, Z.</t>
+  </si>
+  <si>
+    <t>Lifting KK-elements, asymptotic unitary equivalence and classification of simple C∗-algebras.</t>
+  </si>
+  <si>
+    <t>2458153</t>
+  </si>
+  <si>
+    <t>Adv. Math. 219 (2008), no. 5, 1729–1769. </t>
+  </si>
+  <si>
+    <t>Lin, H.</t>
+  </si>
+  <si>
+    <t>Asymptotic unitary equivalence and classification of simple amenable C∗-algebras. </t>
+  </si>
+  <si>
+    <t>Invent. Math. 183 (2011), no. 2, 385–450. </t>
+  </si>
+  <si>
+    <t>2772085</t>
+  </si>
+  <si>
+    <t>Marcoux, Laurent W.; Popov, Alexey I.</t>
+  </si>
+  <si>
+    <t>Abelian, amenable operator algebras are similar to C∗-algebras.</t>
+  </si>
+  <si>
+    <t>Duke Math. J. 165 (2016), no. 12, 2391–2406. </t>
+  </si>
+  <si>
+    <t>3544284</t>
+  </si>
+  <si>
+    <t>(2003) Unpublished manuscript.</t>
+  </si>
+  <si>
+    <t>Non-stable K-theory and extremally rich C∗-algebras</t>
+  </si>
+  <si>
+    <t>J. Funct. Anal. 267 (2014), no. 1, 262–298.</t>
+  </si>
+  <si>
+    <t>3206515</t>
+  </si>
+  <si>
+    <t>Lawrence G. Brown; Gert K. Pedersen</t>
   </si>
 </sst>
 </file>
@@ -802,11 +850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,9 +864,9 @@
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -888,7 +936,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>32</v>
       </c>
@@ -908,7 +956,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>83</v>
       </c>
@@ -1003,7 +1051,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
@@ -1078,7 +1126,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>86</v>
       </c>
@@ -1101,7 +1149,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1173,519 +1221,611 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1971</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <v>1976</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1977</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D19" s="1">
         <v>1977</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E19" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1403992</v>
-      </c>
-      <c r="B18" s="1">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1994</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="1">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2003</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="B20" s="1">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1">
-        <v>2003</v>
+        <v>1979</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1981</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1983</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="1">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>3452230</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="1">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D23" s="1">
-        <v>1971</v>
+        <v>1983</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="B24" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D24" s="1">
-        <v>1977</v>
+        <v>1986</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B25" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D25" s="1">
-        <v>1979</v>
+        <v>1991</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="B26" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D26" s="1">
-        <v>1981</v>
+        <v>1992</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>1403992</v>
       </c>
       <c r="B27" s="1">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1">
-        <v>1983</v>
+        <v>1994</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>148</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>146</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1">
-        <v>1983</v>
+        <v>2001</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1">
-        <v>1986</v>
+        <v>2002</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B30" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="D30" s="1">
-        <v>1991</v>
+        <v>2002</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B31" s="1">
-        <v>12</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D31" s="1">
-        <v>1992</v>
+        <v>2003</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="D32" s="1">
-        <v>2001</v>
+        <v>2003</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>56</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>2188261</v>
       </c>
       <c r="B33" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D33" s="1">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>2188261</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>149</v>
       </c>
       <c r="D34" s="1">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="B35" s="1">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="D35" s="1">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>3452230</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="1">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2013</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>3407494</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B39" s="1">
         <v>18</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D39" s="1">
         <v>2015</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>73</v>
       </c>
     </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:H36">
-    <sortCondition ref="E1"/>
+  <sortState ref="A2:H40">
+    <sortCondition ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>